<commit_message>
Added Sprint 0 Output File and Updated Sprint Report
</commit_message>
<xml_diff>
--- a/TeamBlutUndEisenReport.xlsx
+++ b/TeamBlutUndEisenReport.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarod/cs555/Project_GEDCOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\StevensUser\git_assignments\cs555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2184351C-09C0-402F-AECE-F4B656292265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14496" tabRatio="727" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,10 +22,10 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="189">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -63,9 +62,6 @@
     <t>GitHub Username</t>
   </si>
   <si>
-    <t>jb</t>
-  </si>
-  <si>
     <t>Jarod</t>
   </si>
   <si>
@@ -78,9 +74,6 @@
     <t>jbisnar</t>
   </si>
   <si>
-    <t>mm</t>
-  </si>
-  <si>
     <t>Matthew</t>
   </si>
   <si>
@@ -91,12 +84,6 @@
   </si>
   <si>
     <t>Mmonaco13</t>
-  </si>
-  <si>
-    <t>et</t>
-  </si>
-  <si>
-    <t>Ethat</t>
   </si>
   <si>
     <t>DyTioco</t>
@@ -140,35 +127,16 @@
     <t>Birth before death</t>
   </si>
   <si>
-    <t>hm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Done</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>US05</t>
   </si>
   <si>
     <t>Marriage before death</t>
   </si>
   <si>
-    <t>gh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coding</t>
-  </si>
-  <si>
     <t>US08</t>
   </si>
   <si>
     <t>Birth before marriage</t>
-  </si>
-  <si>
-    <t>at</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>The goal of the burndown chart is to help the agile team and customer to understand how the developers are doing</t>
@@ -269,108 +237,15 @@
     <t>Test lines</t>
   </si>
   <si>
-    <t>gedcom.py</t>
-  </si>
-  <si>
-    <t>us03_birth_b4_death</t>
-  </si>
-  <si>
-    <t>33-36</t>
-  </si>
-  <si>
-    <t>test03.py</t>
-  </si>
-  <si>
-    <t>test_us03</t>
-  </si>
-  <si>
-    <t>15-23</t>
-  </si>
-  <si>
-    <t>T03.01</t>
-  </si>
-  <si>
-    <t>Store birth date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>T03.02</t>
-  </si>
-  <si>
-    <t>Store death date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>T03.03</t>
-  </si>
-  <si>
-    <t>Compare birth and death dates</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coding</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>us05_marr_b4_death</t>
-  </si>
-  <si>
-    <t>test05.py</t>
-  </si>
-  <si>
-    <t>test_us05</t>
-  </si>
-  <si>
-    <t>29-34</t>
-  </si>
-  <si>
-    <t>T05.01</t>
-  </si>
-  <si>
-    <t>Find marriage record for individual</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gh(at)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>T05.02</t>
-  </si>
-  <si>
-    <t>Find marriage date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>T05.03</t>
-  </si>
-  <si>
-    <t>Compare marriage date to birth date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gh(hm)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Review Results</t>
   </si>
   <si>
     <t>Keep doing:</t>
   </si>
   <si>
-    <t>Bring pizza to our meetings</t>
-  </si>
-  <si>
-    <t>Bring silverware for everyone</t>
-  </si>
-  <si>
     <t>Avoid:</t>
   </si>
   <si>
-    <t>Leaving leftover pizza on the counter</t>
-  </si>
-  <si>
     <t>Story ID</t>
   </si>
   <si>
@@ -738,17 +613,32 @@
   </si>
   <si>
     <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
+  </si>
+  <si>
+    <t>JB</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Not Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -795,7 +685,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -805,18 +695,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,7 +776,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -919,9 +797,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -935,8 +810,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="65"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
@@ -1186,10 +1074,7 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40442</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40455</c:v>
+                  <c:v>42263</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1201,10 +1086,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2091,22 +1973,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2123,75 +2005,75 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="19" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D5" s="18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="D9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>21</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
+  <sortState ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{EE78A117-A5BE-F940-AEB7-171D3BEF9F90}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{708BF9A7-32BC-7D49-BD47-EA41552B077F}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{8D81BB70-D1B8-A648-AD8E-888CAC2867CB}"/>
-    <hyperlink ref="E9" r:id="rId4" xr:uid="{D51D1887-2AC5-EA4F-89E9-58A7D3F0320E}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="E9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2199,85 +2081,155 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="8.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="14.1">
-      <c r="A2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="27.95">
-      <c r="A3">
+      <c r="B5" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
+      <c r="B9" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E9" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2288,110 +2240,110 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
+      <c r="E14" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="7" t="s">
+      <c r="F14" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="7" t="s">
+      <c r="G14" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="7" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="7" t="s">
+      <c r="B15" s="12">
+        <v>41065</v>
+      </c>
+      <c r="C15" s="13">
+        <v>24</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1">
-      <c r="A14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="13">
-        <v>41065</v>
-      </c>
-      <c r="C15" s="14">
-        <v>24</v>
-      </c>
-      <c r="E15" s="14">
-        <v>0</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="13">
+      <c r="B16" s="12">
         <v>41078</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="13">
         <v>18</v>
       </c>
       <c r="D16">
         <f>C15-C16</f>
         <v>6</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>250</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="13">
         <v>120</v>
       </c>
       <c r="G16" s="9">
@@ -2399,24 +2351,24 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="13">
+        <v>44</v>
+      </c>
+      <c r="B17" s="12">
         <v>41092</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="13">
         <v>12</v>
       </c>
       <c r="D17">
         <f>C16-C17</f>
         <v>6</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <v>480</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="14">
         <v>135</v>
       </c>
       <c r="G17" s="9">
@@ -2424,24 +2376,24 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="13">
+        <v>45</v>
+      </c>
+      <c r="B18" s="12">
         <v>41106</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="13">
         <v>6</v>
       </c>
       <c r="D18">
         <f>C17-C18</f>
         <v>6</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <v>740</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <v>160</v>
       </c>
       <c r="G18" s="9">
@@ -2449,24 +2401,24 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="13">
+        <v>46</v>
+      </c>
+      <c r="B19" s="12">
         <v>41120</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="13">
         <v>0</v>
       </c>
       <c r="D19">
         <f>C18-C19</f>
         <v>6</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <v>1100</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="14">
         <v>145</v>
       </c>
       <c r="G19" s="9">
@@ -2482,75 +2434,53 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
-        <v>40442</v>
+        <v>42263</v>
       </c>
       <c r="B2">
-        <v>36</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="7">
-        <v>40455</v>
-      </c>
-      <c r="B3">
-        <v>30</v>
-      </c>
-      <c r="C3">
-        <f>B2-B3</f>
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>250</v>
-      </c>
-      <c r="E3">
-        <v>120</v>
-      </c>
-      <c r="F3" s="9">
-        <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
-      </c>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2561,321 +2491,265 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Q21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.125" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.875" style="17" customWidth="1"/>
-    <col min="15" max="15" width="10.125" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.125" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.90625" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.90625" style="16" customWidth="1"/>
+    <col min="15" max="15" width="8.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1796875" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14.1">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="Q1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="E2" s="24">
+        <v>1</v>
+      </c>
+      <c r="F2" s="24">
+        <v>60</v>
+      </c>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="24">
+        <v>5</v>
+      </c>
+      <c r="F3" s="24">
+        <v>120</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="I4" s="7"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="I8" s="7"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="I10" s="7"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="I14" s="7"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="5"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I18" s="7"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="14.1">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2">
-        <v>150</v>
-      </c>
-      <c r="F2">
-        <v>60</v>
-      </c>
-      <c r="G2">
-        <v>120</v>
-      </c>
-      <c r="H2">
-        <v>90</v>
-      </c>
-      <c r="I2" s="7">
-        <v>40444</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="14.1">
-      <c r="A4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:17" ht="14.1">
-      <c r="A5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:17" ht="27.95">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="8" spans="1:17" ht="14.1">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8">
-        <v>200</v>
-      </c>
-      <c r="F8">
-        <v>120</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="K8" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="O8" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="P8" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q8" s="18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="27.95">
-      <c r="A10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:17" ht="14.1">
-      <c r="A11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:17" ht="27.95">
-      <c r="A12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" t="s">
-        <v>91</v>
-      </c>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="14" spans="1:17" ht="14.1">
-      <c r="B14" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="B15" s="5"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:17" ht="14.1">
-      <c r="B16" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="2:2" ht="27.95">
-      <c r="B17" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="27.95">
-      <c r="B18" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="14.1">
-      <c r="B20" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" ht="27.95">
-      <c r="B21" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.95">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2886,42 +2760,42 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.95">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2931,42 +2805,42 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.95">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2976,490 +2850,490 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+    <sheetView topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14.1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C15" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="5" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="33.950000000000003">
-      <c r="A2" t="s">
+      <c r="B16" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C16" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="12" t="s">
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.100000000000001">
-      <c r="A3" t="s">
+      <c r="B17" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="C17" s="22" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.100000000000001">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="12" t="s">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="33.950000000000003">
-      <c r="A5" t="s">
+      <c r="B18" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="C18" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="12" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17.100000000000001">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="B19" s="21" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17.100000000000001">
-      <c r="A7" t="s">
+      <c r="C19" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="21" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="B20" s="21" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="51">
-      <c r="A8" t="s">
+      <c r="C20" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="B21" s="21" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="33.950000000000003">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="21" t="s">
+      <c r="C21" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="12" t="s">
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="33.950000000000003">
-      <c r="A10" t="s">
+      <c r="B22" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="C22" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="12" t="s">
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="33.950000000000003">
-      <c r="A11" t="s">
+      <c r="B23" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C23" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="12" t="s">
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="33.950000000000003">
-      <c r="A12" t="s">
+      <c r="B24" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C24" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="12" t="s">
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="51">
-      <c r="A13" t="s">
+      <c r="B25" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C25" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="C13" s="12" t="s">
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="68.099999999999994">
-      <c r="A14" t="s">
+      <c r="B26" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C26" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="12" t="s">
+    </row>
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="33.950000000000003">
-      <c r="A15" t="s">
+      <c r="B27" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C27" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="C15" s="12" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="21" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="17.100000000000001">
-      <c r="A16" s="20" t="s">
+      <c r="B28" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="C28" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="12" t="s">
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A29" s="21" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="33.950000000000003">
-      <c r="A17" s="20" t="s">
+      <c r="B29" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="C29" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="C17" s="12" t="s">
+    </row>
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="21" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="17.100000000000001">
-      <c r="A18" t="s">
+      <c r="B30" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C30" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="C18" s="12" t="s">
+    </row>
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="21" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="17.100000000000001">
-      <c r="A19" t="s">
+      <c r="B31" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C31" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="C19" s="12" t="s">
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="17.100000000000001">
-      <c r="A20" t="s">
+      <c r="B32" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C32" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="C20" s="12" t="s">
+    </row>
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="21" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="33.950000000000003">
-      <c r="A21" t="s">
+      <c r="B33" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C33" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="12" t="s">
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="33.950000000000003">
-      <c r="A22" s="20" t="s">
+      <c r="B34" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="C34" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="12" t="s">
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="33.950000000000003">
-      <c r="A23" s="20" t="s">
+      <c r="B35" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="C35" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="C23" s="12" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="33.950000000000003">
-      <c r="A24" t="s">
+      <c r="B36" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C36" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="C24" s="12" t="s">
+    </row>
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="51">
-      <c r="A25" t="s">
+      <c r="B37" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C37" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="C25" s="12" t="s">
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A38" s="21" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="33.950000000000003">
-      <c r="A26" t="s">
+      <c r="B38" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C38" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="C26" s="12" t="s">
+    </row>
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A39" s="21" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="135.94999999999999">
-      <c r="A27" t="s">
+      <c r="B39" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C39" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="C27" s="12" t="s">
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A40" s="21" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="17.100000000000001">
-      <c r="A28" s="20" t="s">
+      <c r="B40" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="C40" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="C28" s="12" t="s">
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A41" s="21" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="33.950000000000003">
-      <c r="A29" t="s">
+      <c r="B41" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C41" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="C29" s="12" t="s">
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A42" s="21" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="17.100000000000001">
-      <c r="A30" s="20" t="s">
+      <c r="B42" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="C42" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="C30" s="12" t="s">
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A43" s="21" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="17.100000000000001">
-      <c r="A31" s="20" t="s">
+      <c r="B43" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="C43" s="22" t="s">
         <v>183</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="33.950000000000003">
-      <c r="A32" t="s">
-        <v>185</v>
-      </c>
-      <c r="B32" t="s">
-        <v>186</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="17.100000000000001">
-      <c r="A33" t="s">
-        <v>188</v>
-      </c>
-      <c r="B33" t="s">
-        <v>189</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="33.950000000000003">
-      <c r="A34" t="s">
-        <v>191</v>
-      </c>
-      <c r="B34" t="s">
-        <v>192</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="51">
-      <c r="A35" t="s">
-        <v>194</v>
-      </c>
-      <c r="B35" t="s">
-        <v>195</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="33.950000000000003">
-      <c r="A36" t="s">
-        <v>197</v>
-      </c>
-      <c r="B36" t="s">
-        <v>198</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="33.950000000000003">
-      <c r="A37" t="s">
-        <v>200</v>
-      </c>
-      <c r="B37" t="s">
-        <v>201</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="33.950000000000003">
-      <c r="A38" t="s">
-        <v>203</v>
-      </c>
-      <c r="B38" t="s">
-        <v>204</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="33.950000000000003">
-      <c r="A39" t="s">
-        <v>206</v>
-      </c>
-      <c r="B39" t="s">
-        <v>207</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="33.950000000000003">
-      <c r="A40" t="s">
-        <v>209</v>
-      </c>
-      <c r="B40" t="s">
-        <v>210</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="33.950000000000003">
-      <c r="A41" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="33.950000000000003">
-      <c r="A42" t="s">
-        <v>215</v>
-      </c>
-      <c r="B42" t="s">
-        <v>216</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="33.950000000000003">
-      <c r="A43" t="s">
-        <v>218</v>
-      </c>
-      <c r="B43" t="s">
-        <v>219</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Sprint1 plans for JB edited MM's est size
</commit_message>
<xml_diff>
--- a/TeamBlutUndEisenReport.xlsx
+++ b/TeamBlutUndEisenReport.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\StevensUser\git_assignments\cs555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jarod/cs555/Project_GEDCOM/cs555/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D0C6CB-1980-C841-9F5E-4E66480ECFD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14496" tabRatio="727" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380" tabRatio="727" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="189">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -633,7 +634,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -934,7 +935,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1005,7 +1006,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1973,22 +1974,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>184</v>
       </c>
@@ -2022,7 +2023,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>185</v>
       </c>
@@ -2039,7 +2040,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>186</v>
       </c>
@@ -2056,7 +2057,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
@@ -2065,15 +2066,15 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:D5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="E9" r:id="rId4"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2081,23 +2082,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -2114,7 +2115,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B2" s="21" t="s">
         <v>100</v>
       </c>
@@ -2128,7 +2129,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B3" s="21" t="s">
         <v>103</v>
       </c>
@@ -2142,7 +2143,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" s="21" t="s">
         <v>118</v>
       </c>
@@ -2156,7 +2157,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2173,7 +2174,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" s="21" t="s">
         <v>136</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B7" s="21" t="s">
         <v>142</v>
       </c>
@@ -2201,7 +2202,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B8" s="21" t="s">
         <v>145</v>
       </c>
@@ -2215,7 +2216,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2240,54 +2241,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
@@ -2310,7 +2311,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -2326,7 +2327,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2351,7 +2352,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>44</v>
       </c>
@@ -2376,7 +2377,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>45</v>
       </c>
@@ -2401,7 +2402,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -2434,24 +2435,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="2"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="7.08984375" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="7">
         <v>42263</v>
       </c>
@@ -2479,7 +2480,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="7"/>
     </row>
   </sheetData>
@@ -2491,34 +2492,34 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB22"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.08984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.36328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.90625" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.81640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.90625" style="16" customWidth="1"/>
-    <col min="15" max="15" width="8.1796875" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.6328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" style="16" customWidth="1"/>
+    <col min="15" max="15" width="8.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2565,7 +2566,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A2" s="23" t="s">
         <v>121</v>
       </c>
@@ -2579,7 +2580,7 @@
         <v>188</v>
       </c>
       <c r="E2" s="24">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F2" s="24">
         <v>60</v>
@@ -2607,7 +2608,7 @@
       <c r="AA2" s="23"/>
       <c r="AB2" s="23"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A3" s="21" t="s">
         <v>175</v>
       </c>
@@ -2621,7 +2622,7 @@
         <v>188</v>
       </c>
       <c r="E3" s="24">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="F3" s="24">
         <v>120</v>
@@ -2649,7 +2650,25 @@
       <c r="AA3" s="23"/>
       <c r="AB3" s="23"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="14" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
       <c r="I4" s="7"/>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
@@ -2658,16 +2677,36 @@
       <c r="P4" s="17"/>
       <c r="Q4" s="17"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
       <c r="I8" s="7"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
       <c r="I10" s="7"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
@@ -2676,32 +2715,32 @@
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
       <c r="I14" s="7"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="14" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>58</v>
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B17" s="5"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="5" t="s">
         <v>59</v>
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="5" t="s">
         <v>60</v>
       </c>
@@ -2714,16 +2753,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2760,16 +2799,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2805,16 +2844,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2850,20 +2889,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="109" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A41" sqref="A41:B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="19" t="s">
         <v>61</v>
       </c>
@@ -2874,7 +2913,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="21" t="s">
         <v>64</v>
       </c>
@@ -2885,7 +2924,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" s="21" t="s">
         <v>67</v>
       </c>
@@ -2896,7 +2935,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="21" t="s">
         <v>23</v>
       </c>
@@ -2907,7 +2946,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" s="21" t="s">
         <v>70</v>
       </c>
@@ -2918,7 +2957,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" s="21" t="s">
         <v>25</v>
       </c>
@@ -2929,7 +2968,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="21" t="s">
         <v>74</v>
       </c>
@@ -2940,7 +2979,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" s="21" t="s">
         <v>77</v>
       </c>
@@ -2951,7 +2990,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" s="21" t="s">
         <v>27</v>
       </c>
@@ -2962,7 +3001,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" s="21" t="s">
         <v>82</v>
       </c>
@@ -2973,7 +3012,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" s="21" t="s">
         <v>85</v>
       </c>
@@ -2984,7 +3023,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" s="21" t="s">
         <v>88</v>
       </c>
@@ -2995,7 +3034,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" s="21" t="s">
         <v>91</v>
       </c>
@@ -3006,7 +3045,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" s="21" t="s">
         <v>94</v>
       </c>
@@ -3017,7 +3056,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" s="21" t="s">
         <v>97</v>
       </c>
@@ -3028,7 +3067,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" s="21" t="s">
         <v>100</v>
       </c>
@@ -3039,7 +3078,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" s="21" t="s">
         <v>103</v>
       </c>
@@ -3050,7 +3089,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" s="21" t="s">
         <v>106</v>
       </c>
@@ -3061,7 +3100,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="21" t="s">
         <v>109</v>
       </c>
@@ -3072,7 +3111,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" s="21" t="s">
         <v>112</v>
       </c>
@@ -3083,7 +3122,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" s="21" t="s">
         <v>115</v>
       </c>
@@ -3094,7 +3133,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" s="21" t="s">
         <v>118</v>
       </c>
@@ -3105,7 +3144,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" s="21" t="s">
         <v>121</v>
       </c>
@@ -3116,7 +3155,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" s="21" t="s">
         <v>124</v>
       </c>
@@ -3127,7 +3166,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" s="21" t="s">
         <v>127</v>
       </c>
@@ -3138,7 +3177,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" s="21" t="s">
         <v>130</v>
       </c>
@@ -3149,7 +3188,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" s="21" t="s">
         <v>133</v>
       </c>
@@ -3160,7 +3199,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" s="21" t="s">
         <v>136</v>
       </c>
@@ -3171,7 +3210,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" s="21" t="s">
         <v>139</v>
       </c>
@@ -3182,7 +3221,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="21" t="s">
         <v>142</v>
       </c>
@@ -3193,7 +3232,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" s="21" t="s">
         <v>145</v>
       </c>
@@ -3204,7 +3243,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" s="21" t="s">
         <v>148</v>
       </c>
@@ -3215,7 +3254,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" s="21" t="s">
         <v>151</v>
       </c>
@@ -3226,7 +3265,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" s="21" t="s">
         <v>154</v>
       </c>
@@ -3237,7 +3276,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" s="21" t="s">
         <v>157</v>
       </c>
@@ -3248,7 +3287,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" s="21" t="s">
         <v>160</v>
       </c>
@@ -3259,7 +3298,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" s="21" t="s">
         <v>163</v>
       </c>
@@ -3270,7 +3309,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" s="21" t="s">
         <v>166</v>
       </c>
@@ -3281,7 +3320,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" s="21" t="s">
         <v>169</v>
       </c>
@@ -3292,7 +3331,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" s="21" t="s">
         <v>172</v>
       </c>
@@ -3303,7 +3342,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" s="21" t="s">
         <v>175</v>
       </c>
@@ -3314,7 +3353,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" s="21" t="s">
         <v>178</v>
       </c>
@@ -3325,7 +3364,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" s="21" t="s">
         <v>181</v>
       </c>

</xml_diff>

<commit_message>
added Sprint1 plans for ED
</commit_message>
<xml_diff>
--- a/TeamBlutUndEisenReport.xlsx
+++ b/TeamBlutUndEisenReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jarod/cs555/Project_GEDCOM/cs555/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\cs555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D0C6CB-1980-C841-9F5E-4E66480ECFD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F6EE6C-C9FE-4960-BB4C-CA4453CDB3C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380" tabRatio="727" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="727" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="191">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -629,6 +631,12 @@
   </si>
   <si>
     <t>Not Done</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Less than 100 years old</t>
   </si>
 </sst>
 </file>
@@ -777,7 +785,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -826,6 +834,10 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
@@ -935,7 +947,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1006,7 +1018,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1981,15 +1993,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2006,7 +2018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>184</v>
       </c>
@@ -2023,7 +2035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>185</v>
       </c>
@@ -2040,7 +2052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>186</v>
       </c>
@@ -2057,7 +2069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
@@ -2086,19 +2098,19 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -2115,7 +2127,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" s="21" t="s">
         <v>100</v>
       </c>
@@ -2129,7 +2141,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="21" t="s">
         <v>103</v>
       </c>
@@ -2143,7 +2155,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="21" t="s">
         <v>118</v>
       </c>
@@ -2157,7 +2169,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2174,7 +2186,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="21" t="s">
         <v>136</v>
       </c>
@@ -2188,7 +2200,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
         <v>142</v>
       </c>
@@ -2202,7 +2214,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="21" t="s">
         <v>145</v>
       </c>
@@ -2216,7 +2228,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2244,51 +2256,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
@@ -2311,7 +2323,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -2327,7 +2339,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2352,7 +2364,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>44</v>
       </c>
@@ -2377,7 +2389,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>45</v>
       </c>
@@ -2402,7 +2414,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -2442,17 +2454,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -2472,7 +2484,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>42263</v>
       </c>
@@ -2480,7 +2492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
     </row>
   </sheetData>
@@ -2495,31 +2507,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="8.1640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.81640625" style="16" customWidth="1"/>
+    <col min="15" max="15" width="8.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1796875" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2566,7 +2578,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>121</v>
       </c>
@@ -2608,7 +2620,7 @@
       <c r="AA2" s="23"/>
       <c r="AB2" s="23"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>175</v>
       </c>
@@ -2650,7 +2662,7 @@
       <c r="AA3" s="23"/>
       <c r="AB3" s="23"/>
     </row>
-    <row r="4" spans="1:28" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -2677,7 +2689,7 @@
       <c r="P4" s="17"/>
       <c r="Q4" s="17"/>
     </row>
-    <row r="5" spans="1:28" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2697,16 +2709,52 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>70</v>
+      </c>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" t="s">
+        <v>188</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>70</v>
+      </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I8" s="7"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I10" s="7"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
@@ -2715,32 +2763,32 @@
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I14" s="7"/>
     </row>
-    <row r="16" spans="1:28" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>58</v>
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>59</v>
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="22" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>60</v>
       </c>
@@ -2760,9 +2808,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2806,9 +2854,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2851,9 +2899,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2890,19 +2938,19 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView zoomScale="109" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:B41"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>61</v>
       </c>
@@ -2912,8 +2960,11 @@
       <c r="C1" s="20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>64</v>
       </c>
@@ -2923,8 +2974,11 @@
       <c r="C2" s="22" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>67</v>
       </c>
@@ -2934,8 +2988,11 @@
       <c r="C3" s="22" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>23</v>
       </c>
@@ -2945,8 +3002,11 @@
       <c r="C4" s="22" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>70</v>
       </c>
@@ -2956,8 +3016,11 @@
       <c r="C5" s="22" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>25</v>
       </c>
@@ -2967,8 +3030,11 @@
       <c r="C6" s="22" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>74</v>
       </c>
@@ -2978,8 +3044,11 @@
       <c r="C7" s="22" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>77</v>
       </c>
@@ -2989,8 +3058,11 @@
       <c r="C8" s="22" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="27"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>27</v>
       </c>
@@ -3000,8 +3072,11 @@
       <c r="C9" s="22" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>82</v>
       </c>
@@ -3011,8 +3086,11 @@
       <c r="C10" s="22" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>85</v>
       </c>
@@ -3022,8 +3100,11 @@
       <c r="C11" s="22" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>88</v>
       </c>
@@ -3033,8 +3114,11 @@
       <c r="C12" s="22" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
         <v>91</v>
       </c>
@@ -3044,8 +3128,11 @@
       <c r="C13" s="22" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>94</v>
       </c>
@@ -3055,8 +3142,11 @@
       <c r="C14" s="22" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>97</v>
       </c>
@@ -3066,8 +3156,11 @@
       <c r="C15" s="22" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
         <v>100</v>
       </c>
@@ -3077,8 +3170,11 @@
       <c r="C16" s="22" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>103</v>
       </c>
@@ -3088,8 +3184,11 @@
       <c r="C17" s="22" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>106</v>
       </c>
@@ -3099,8 +3198,11 @@
       <c r="C18" s="22" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
         <v>109</v>
       </c>
@@ -3110,8 +3212,11 @@
       <c r="C19" s="22" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>112</v>
       </c>
@@ -3121,8 +3226,11 @@
       <c r="C20" s="22" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="s">
         <v>115</v>
       </c>
@@ -3132,8 +3240,11 @@
       <c r="C21" s="22" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="s">
         <v>118</v>
       </c>
@@ -3143,8 +3254,11 @@
       <c r="C22" s="22" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
         <v>121</v>
       </c>
@@ -3154,8 +3268,11 @@
       <c r="C23" s="22" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
         <v>124</v>
       </c>
@@ -3165,8 +3282,11 @@
       <c r="C24" s="22" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
         <v>127</v>
       </c>
@@ -3176,8 +3296,11 @@
       <c r="C25" s="22" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
         <v>130</v>
       </c>
@@ -3187,8 +3310,11 @@
       <c r="C26" s="22" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="1:6" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
         <v>133</v>
       </c>
@@ -3198,8 +3324,11 @@
       <c r="C27" s="22" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+    </row>
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
         <v>136</v>
       </c>
@@ -3209,8 +3338,11 @@
       <c r="C28" s="22" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
         <v>139</v>
       </c>
@@ -3220,8 +3352,11 @@
       <c r="C29" s="22" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
         <v>142</v>
       </c>
@@ -3231,8 +3366,11 @@
       <c r="C30" s="22" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="s">
         <v>145</v>
       </c>
@@ -3242,8 +3380,11 @@
       <c r="C31" s="22" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
         <v>148</v>
       </c>
@@ -3253,8 +3394,11 @@
       <c r="C32" s="22" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+    </row>
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="s">
         <v>151</v>
       </c>
@@ -3264,8 +3408,11 @@
       <c r="C33" s="22" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
         <v>154</v>
       </c>
@@ -3275,8 +3422,11 @@
       <c r="C34" s="22" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>157</v>
       </c>
@@ -3286,8 +3436,11 @@
       <c r="C35" s="22" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>160</v>
       </c>
@@ -3297,8 +3450,11 @@
       <c r="C36" s="22" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+    </row>
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
         <v>163</v>
       </c>
@@ -3308,8 +3464,11 @@
       <c r="C37" s="22" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
         <v>166</v>
       </c>
@@ -3319,8 +3478,11 @@
       <c r="C38" s="22" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
         <v>169</v>
       </c>
@@ -3330,8 +3492,11 @@
       <c r="C39" s="22" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
         <v>172</v>
       </c>
@@ -3341,8 +3506,11 @@
       <c r="C40" s="22" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+    </row>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="s">
         <v>175</v>
       </c>
@@ -3352,8 +3520,11 @@
       <c r="C41" s="22" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
         <v>178</v>
       </c>
@@ -3363,8 +3534,11 @@
       <c r="C42" s="22" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+    </row>
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
         <v>181</v>
       </c>
@@ -3374,6 +3548,9 @@
       <c r="C43" s="22" t="s">
         <v>183</v>
       </c>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated backlog, and added ED's part for Sprint1
</commit_message>
<xml_diff>
--- a/TeamBlutUndEisenReport.xlsx
+++ b/TeamBlutUndEisenReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\cs555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F6EE6C-C9FE-4960-BB4C-CA4453CDB3C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3104FFA-A2EC-4ED0-97D4-8FDB82AF1A63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="727" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="727" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="191">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2095,17 +2095,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6328125" customWidth="1"/>
     <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2242,6 +2242,242 @@
         <v>185</v>
       </c>
       <c r="E9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>184</v>
+      </c>
+      <c r="E13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>184</v>
+      </c>
+      <c r="E14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
+        <v>184</v>
+      </c>
+      <c r="E15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" t="s">
+        <v>184</v>
+      </c>
+      <c r="E16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
+        <v>184</v>
+      </c>
+      <c r="E17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" t="s">
+        <v>189</v>
+      </c>
+      <c r="E20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" t="s">
+        <v>189</v>
+      </c>
+      <c r="E21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" t="s">
+        <v>189</v>
+      </c>
+      <c r="E22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="s">
+        <v>189</v>
+      </c>
+      <c r="E23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" t="s">
+        <v>189</v>
+      </c>
+      <c r="E24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D25" t="s">
+        <v>189</v>
+      </c>
+      <c r="E25" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2508,7 +2744,7 @@
   <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2940,8 +3176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A40" zoomScale="109" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>

</xml_diff>